<commit_message>
changed maximum capacity of treatment unit to match thoeritical maximum capacity of mee-mvr
</commit_message>
<xml_diff>
--- a/pareto/case_studies/integrated_desalination_case_study.xlsx
+++ b/pareto/case_studies/integrated_desalination_case_study.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssnaik\Biegler\PARETO\pyomo_models\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4756B6E6-A44A-46AD-B77E-171770CF4335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3AF109-DCAE-4EE5-8ECC-956329029FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="834" firstSheet="80" activeTab="85" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -4624,7 +4624,7 @@
   <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5902,7 +5902,7 @@
   <dimension ref="A1:BA10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8466,7 +8466,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8510,7 +8510,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8538,7 +8538,7 @@
         <v>119</v>
       </c>
       <c r="B3" s="71">
-        <v>10000</v>
+        <v>10868.8</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -8546,7 +8546,7 @@
         <v>120</v>
       </c>
       <c r="B4" s="43">
-        <v>20000</v>
+        <v>10868.8</v>
       </c>
     </row>
   </sheetData>
@@ -10011,7 +10011,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11292,7 +11292,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -14285,7 +14285,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changes with USD as cost units
</commit_message>
<xml_diff>
--- a/pareto/case_studies/integrated_desalination_case_study.xlsx
+++ b/pareto/case_studies/integrated_desalination_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssnaik\Biegler\PARETO\pyomo_models\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3AF109-DCAE-4EE5-8ECC-956329029FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC39388-6201-4C55-BEDE-606C75EF8327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="834" firstSheet="80" activeTab="85" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="834" firstSheet="55" activeTab="56" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -931,9 +931,6 @@
     <t>Time discretization for inventory</t>
   </si>
   <si>
-    <t>Cost to store produced water [kUSD/bbl]</t>
-  </si>
-  <si>
     <t>Cost to release produced water [kUSD/bbl]</t>
   </si>
   <si>
@@ -947,6 +944,9 @@
   </si>
   <si>
     <t>Table of Initial Storage Capacity [liters]</t>
+  </si>
+  <si>
+    <t>Cost to store produced water [USD/bbl]</t>
   </si>
 </sst>
 </file>
@@ -3612,7 +3612,9 @@
   </sheetPr>
   <dimension ref="C3:M36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3725,7 +3727,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4483,7 +4485,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4624,7 +4626,7 @@
   <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4774,7 +4776,7 @@
         <v>68</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7" s="56" t="s">
         <v>70</v>
@@ -5048,7 +5050,9 @@
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5196,7 +5200,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5248,7 +5252,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5323,7 +5327,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6957,7 +6961,7 @@
   </sheetPr>
   <dimension ref="A1:BA6"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -7391,7 +7395,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8472,12 +8476,13 @@
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -8510,7 +8515,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8563,7 +8568,7 @@
   <dimension ref="A1:BA15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9488,7 +9493,7 @@
   <dimension ref="A1:BA9"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10011,7 +10016,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10023,7 +10028,7 @@
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Disposal Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Disposal Operational Cost [kUSD/bbl]</v>
+        <v>Table of Disposal Operational Cost [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -10039,8 +10044,8 @@
         <v>111</v>
       </c>
       <c r="B3" s="29">
-        <f>0.35*0.001</f>
-        <v>3.5E-4</v>
+        <f>0.35</f>
+        <v>0.35</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -10048,8 +10053,8 @@
         <v>112</v>
       </c>
       <c r="B4" s="29">
-        <f>0.35*0.001</f>
-        <v>3.5E-4</v>
+        <f>0.35</f>
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>
@@ -10067,7 +10072,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10079,7 +10084,7 @@
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Treatment Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Treatment Operational Cost [kUSD/bbl]</v>
+        <v>Table of Treatment Operational Cost [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -10094,18 +10099,16 @@
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="32">
-        <f>0.001*0.5</f>
-        <v>5.0000000000000001E-4</v>
+      <c r="B3" s="29">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="32">
-        <f>0.001*0.2</f>
-        <v>2.0000000000000001E-4</v>
+      <c r="B4" s="29">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -10121,7 +10124,9 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10132,7 +10137,7 @@
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Reuse Operational Cost [kUSD/bbl]</v>
+        <v>Table of Reuse Operational Cost [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -10164,8 +10169,8 @@
   </sheetPr>
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10193,7 +10198,7 @@
     <row r="1" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Pipeline Operational Cost between Sites [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Pipeline Operational Cost between Sites [kUSD/bbl]</v>
+        <v>Table of Pipeline Operational Cost between Sites [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -10250,49 +10255,49 @@
       <c r="A3" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="C3" s="109">
-        <v>0</v>
-      </c>
-      <c r="D3" s="109">
-        <v>0</v>
-      </c>
-      <c r="E3" s="109">
-        <v>0</v>
-      </c>
-      <c r="F3" s="109">
-        <v>0</v>
-      </c>
-      <c r="G3" s="109">
-        <v>0</v>
-      </c>
-      <c r="H3" s="109">
-        <v>0</v>
-      </c>
-      <c r="I3" s="109">
-        <v>0</v>
-      </c>
-      <c r="J3" s="109">
-        <v>0</v>
-      </c>
-      <c r="K3" s="109">
-        <v>0</v>
-      </c>
-      <c r="L3" s="109">
-        <v>0</v>
-      </c>
-      <c r="M3" s="109">
-        <v>0</v>
-      </c>
-      <c r="N3" s="109">
-        <v>0</v>
-      </c>
-      <c r="O3" s="109">
-        <v>0</v>
-      </c>
-      <c r="P3" s="109">
+      <c r="B3" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
         <v>0</v>
       </c>
     </row>
@@ -10300,49 +10305,49 @@
       <c r="A4" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="109">
-        <v>0</v>
-      </c>
-      <c r="C4" s="109">
-        <v>0</v>
-      </c>
-      <c r="D4" s="109">
-        <v>0</v>
-      </c>
-      <c r="E4" s="109">
-        <v>0</v>
-      </c>
-      <c r="F4" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="G4" s="109">
-        <v>0</v>
-      </c>
-      <c r="H4" s="109">
-        <v>0</v>
-      </c>
-      <c r="I4" s="109">
-        <v>0</v>
-      </c>
-      <c r="J4" s="109">
-        <v>0</v>
-      </c>
-      <c r="K4" s="109">
-        <v>0</v>
-      </c>
-      <c r="L4" s="109">
-        <v>0</v>
-      </c>
-      <c r="M4" s="109">
-        <v>0</v>
-      </c>
-      <c r="N4" s="109">
-        <v>0</v>
-      </c>
-      <c r="O4" s="109">
-        <v>0</v>
-      </c>
-      <c r="P4" s="109">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
         <v>0</v>
       </c>
     </row>
@@ -10350,49 +10355,49 @@
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="109">
-        <v>0</v>
-      </c>
-      <c r="C5" s="109">
-        <v>0</v>
-      </c>
-      <c r="D5" s="109">
-        <v>0</v>
-      </c>
-      <c r="E5" s="109">
-        <v>0</v>
-      </c>
-      <c r="F5" s="109">
-        <v>0</v>
-      </c>
-      <c r="G5" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="H5" s="109">
-        <v>0</v>
-      </c>
-      <c r="I5" s="109">
-        <v>0</v>
-      </c>
-      <c r="J5" s="109">
-        <v>0</v>
-      </c>
-      <c r="K5" s="109">
-        <v>0</v>
-      </c>
-      <c r="L5" s="109">
-        <v>0</v>
-      </c>
-      <c r="M5" s="109">
-        <v>0</v>
-      </c>
-      <c r="N5" s="109">
-        <v>0</v>
-      </c>
-      <c r="O5" s="109">
-        <v>0</v>
-      </c>
-      <c r="P5" s="109">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
         <v>0</v>
       </c>
     </row>
@@ -10400,49 +10405,49 @@
       <c r="A6" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="109">
-        <v>0</v>
-      </c>
-      <c r="C6" s="109">
-        <v>0</v>
-      </c>
-      <c r="D6" s="109">
-        <v>0</v>
-      </c>
-      <c r="E6" s="109">
-        <v>0</v>
-      </c>
-      <c r="F6" s="109">
-        <v>0</v>
-      </c>
-      <c r="G6" s="109">
-        <v>0</v>
-      </c>
-      <c r="H6" s="109">
-        <v>0</v>
-      </c>
-      <c r="I6" s="109">
-        <v>0</v>
-      </c>
-      <c r="J6" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="K6" s="109">
-        <v>0</v>
-      </c>
-      <c r="L6" s="109">
-        <v>0</v>
-      </c>
-      <c r="M6" s="109">
-        <v>0</v>
-      </c>
-      <c r="N6" s="109">
-        <v>0</v>
-      </c>
-      <c r="O6" s="109">
-        <v>0</v>
-      </c>
-      <c r="P6" s="109">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
         <v>0</v>
       </c>
     </row>
@@ -10450,49 +10455,49 @@
       <c r="A7" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="C7" s="109">
-        <v>0</v>
-      </c>
-      <c r="D7" s="109">
-        <v>0</v>
-      </c>
-      <c r="E7" s="109">
-        <v>0</v>
-      </c>
-      <c r="F7" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="G7" s="109">
-        <v>0</v>
-      </c>
-      <c r="H7" s="109">
-        <v>0</v>
-      </c>
-      <c r="I7" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="J7" s="109">
-        <v>0</v>
-      </c>
-      <c r="K7" s="109">
-        <v>0</v>
-      </c>
-      <c r="L7" s="109">
-        <v>0</v>
-      </c>
-      <c r="M7" s="109">
-        <v>0</v>
-      </c>
-      <c r="N7" s="109">
-        <v>0</v>
-      </c>
-      <c r="O7" s="109">
-        <v>0</v>
-      </c>
-      <c r="P7" s="109">
+      <c r="B7" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
         <v>0</v>
       </c>
       <c r="R7" s="109"/>
@@ -10501,99 +10506,99 @@
       <c r="A8" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="109">
-        <v>0</v>
-      </c>
-      <c r="C8" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="D8" s="109">
-        <v>0</v>
-      </c>
-      <c r="E8" s="109">
-        <v>0</v>
-      </c>
-      <c r="F8" s="109">
-        <v>0</v>
-      </c>
-      <c r="G8" s="109">
-        <v>0</v>
-      </c>
-      <c r="H8" s="109">
-        <v>0</v>
-      </c>
-      <c r="I8" s="109">
-        <v>0</v>
-      </c>
-      <c r="J8" s="109">
-        <v>0</v>
-      </c>
-      <c r="K8" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="L8" s="109">
-        <v>0</v>
-      </c>
-      <c r="M8" s="109">
-        <v>0</v>
-      </c>
-      <c r="N8" s="109">
-        <v>0</v>
-      </c>
-      <c r="O8" s="109">
-        <v>0</v>
-      </c>
-      <c r="P8" s="109">
-        <v>1.0000000000000002E-6</v>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="C9" s="109">
-        <v>0</v>
-      </c>
-      <c r="D9" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="E9" s="109">
-        <v>0</v>
-      </c>
-      <c r="F9" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="G9" s="109">
-        <v>0</v>
-      </c>
-      <c r="H9" s="109">
-        <v>0</v>
-      </c>
-      <c r="I9" s="109">
-        <v>0</v>
-      </c>
-      <c r="J9" s="109">
-        <v>0</v>
-      </c>
-      <c r="K9" s="109">
-        <v>0</v>
-      </c>
-      <c r="L9" s="109">
-        <v>0</v>
-      </c>
-      <c r="M9" s="109">
-        <v>0</v>
-      </c>
-      <c r="N9" s="109">
-        <v>0</v>
-      </c>
-      <c r="O9" s="109">
-        <v>0</v>
-      </c>
-      <c r="P9" s="109">
+      <c r="B9" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
         <v>0</v>
       </c>
     </row>
@@ -10601,49 +10606,49 @@
       <c r="A10" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="109">
-        <v>0</v>
-      </c>
-      <c r="C10" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="D10" s="109">
-        <v>0</v>
-      </c>
-      <c r="E10" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="F10" s="109">
-        <v>0</v>
-      </c>
-      <c r="G10" s="109">
-        <v>0</v>
-      </c>
-      <c r="H10" s="109">
-        <v>0</v>
-      </c>
-      <c r="I10" s="109">
-        <v>0</v>
-      </c>
-      <c r="J10" s="109">
-        <v>0</v>
-      </c>
-      <c r="K10" s="109">
-        <v>0</v>
-      </c>
-      <c r="L10" s="109">
-        <v>0</v>
-      </c>
-      <c r="M10" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="N10" s="109">
-        <v>0</v>
-      </c>
-      <c r="O10" s="109">
-        <v>0</v>
-      </c>
-      <c r="P10" s="109">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
         <v>0</v>
       </c>
       <c r="R10" s="109"/>
@@ -10652,49 +10657,49 @@
       <c r="A11" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="109">
-        <v>0</v>
-      </c>
-      <c r="C11" s="109">
-        <v>0</v>
-      </c>
-      <c r="D11" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="E11" s="109">
-        <v>0</v>
-      </c>
-      <c r="F11" s="109">
-        <v>0</v>
-      </c>
-      <c r="G11" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="H11" s="109">
-        <v>0</v>
-      </c>
-      <c r="I11" s="109">
-        <v>0</v>
-      </c>
-      <c r="J11" s="109">
-        <v>0</v>
-      </c>
-      <c r="K11" s="109">
-        <v>0</v>
-      </c>
-      <c r="L11" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="M11" s="109">
-        <v>0</v>
-      </c>
-      <c r="N11" s="109">
-        <v>0</v>
-      </c>
-      <c r="O11" s="109">
-        <v>0</v>
-      </c>
-      <c r="P11" s="109">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
         <v>0</v>
       </c>
     </row>
@@ -10702,99 +10707,99 @@
       <c r="A12" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="109">
-        <v>0</v>
-      </c>
-      <c r="C12" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="D12" s="109">
-        <v>0</v>
-      </c>
-      <c r="E12" s="109">
-        <v>0</v>
-      </c>
-      <c r="F12" s="109">
-        <v>0</v>
-      </c>
-      <c r="G12" s="109">
-        <v>0</v>
-      </c>
-      <c r="H12" s="109">
-        <v>0</v>
-      </c>
-      <c r="I12" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="J12" s="109">
-        <v>0</v>
-      </c>
-      <c r="K12" s="109">
-        <v>0</v>
-      </c>
-      <c r="L12" s="109">
-        <v>0</v>
-      </c>
-      <c r="M12" s="109">
-        <v>0</v>
-      </c>
-      <c r="N12" s="109">
-        <v>0</v>
-      </c>
-      <c r="O12" s="109">
-        <v>0</v>
-      </c>
-      <c r="P12" s="109">
-        <v>1.0000000000000002E-6</v>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="109">
-        <v>0</v>
-      </c>
-      <c r="C13" s="109">
-        <v>0</v>
-      </c>
-      <c r="D13" s="109">
-        <v>0</v>
-      </c>
-      <c r="E13" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="F13" s="109">
-        <v>0</v>
-      </c>
-      <c r="G13" s="109">
-        <v>0</v>
-      </c>
-      <c r="H13" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="I13" s="109">
-        <v>0</v>
-      </c>
-      <c r="J13" s="109">
-        <v>0</v>
-      </c>
-      <c r="K13" s="109">
-        <v>0</v>
-      </c>
-      <c r="L13" s="109">
-        <v>0</v>
-      </c>
-      <c r="M13" s="109">
-        <v>0</v>
-      </c>
-      <c r="N13" s="109">
-        <v>0</v>
-      </c>
-      <c r="O13" s="109">
-        <v>0</v>
-      </c>
-      <c r="P13" s="109">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
         <v>0</v>
       </c>
     </row>
@@ -10802,49 +10807,49 @@
       <c r="A14" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="109">
-        <v>0</v>
-      </c>
-      <c r="C14" s="109">
-        <v>0</v>
-      </c>
-      <c r="D14" s="109">
-        <v>0</v>
-      </c>
-      <c r="E14" s="109">
-        <v>0</v>
-      </c>
-      <c r="F14" s="109">
-        <v>0</v>
-      </c>
-      <c r="G14" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="H14" s="109">
-        <v>0</v>
-      </c>
-      <c r="I14" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="J14" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="K14" s="109">
-        <v>0</v>
-      </c>
-      <c r="L14" s="109">
-        <v>0</v>
-      </c>
-      <c r="M14" s="109">
-        <v>0</v>
-      </c>
-      <c r="N14" s="109">
-        <v>0</v>
-      </c>
-      <c r="O14" s="109">
-        <v>0</v>
-      </c>
-      <c r="P14" s="109">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
         <v>0</v>
       </c>
     </row>
@@ -10852,49 +10857,49 @@
       <c r="A15" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="109">
-        <v>0</v>
-      </c>
-      <c r="C15" s="109">
-        <v>0</v>
-      </c>
-      <c r="D15" s="109">
-        <v>0</v>
-      </c>
-      <c r="E15" s="109">
-        <v>0</v>
-      </c>
-      <c r="F15" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="G15" s="109">
-        <v>0</v>
-      </c>
-      <c r="H15" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="I15" s="109">
-        <v>0</v>
-      </c>
-      <c r="J15" s="109">
-        <v>0</v>
-      </c>
-      <c r="K15" s="109">
-        <v>0</v>
-      </c>
-      <c r="L15" s="109">
-        <v>0</v>
-      </c>
-      <c r="M15" s="109">
-        <v>0</v>
-      </c>
-      <c r="N15" s="109">
-        <v>0</v>
-      </c>
-      <c r="O15" s="109">
-        <v>0</v>
-      </c>
-      <c r="P15" s="109">
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0</v>
+      </c>
+      <c r="P15" s="1">
         <v>0</v>
       </c>
     </row>
@@ -10902,49 +10907,49 @@
       <c r="A16" s="70" t="s">
         <v>133</v>
       </c>
-      <c r="B16" s="109">
-        <v>0</v>
-      </c>
-      <c r="C16" s="109">
-        <v>0</v>
-      </c>
-      <c r="D16" s="109">
-        <v>0</v>
-      </c>
-      <c r="E16" s="109">
-        <v>0</v>
-      </c>
-      <c r="F16" s="109">
-        <v>0</v>
-      </c>
-      <c r="G16" s="109">
-        <v>0</v>
-      </c>
-      <c r="H16" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="I16" s="109">
-        <v>0</v>
-      </c>
-      <c r="J16" s="109">
-        <v>0</v>
-      </c>
-      <c r="K16" s="109">
-        <v>0</v>
-      </c>
-      <c r="L16" s="109">
-        <v>0</v>
-      </c>
-      <c r="M16" s="109">
-        <v>0</v>
-      </c>
-      <c r="N16" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="O16" s="109">
-        <v>0</v>
-      </c>
-      <c r="P16" s="109">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
         <v>0</v>
       </c>
       <c r="Q16" s="109"/>
@@ -10953,199 +10958,199 @@
       <c r="A17" s="70" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="109">
-        <v>0</v>
-      </c>
-      <c r="C17" s="109">
-        <v>0</v>
-      </c>
-      <c r="D17" s="109">
-        <v>0</v>
-      </c>
-      <c r="E17" s="109">
-        <v>0</v>
-      </c>
-      <c r="F17" s="109">
-        <v>0</v>
-      </c>
-      <c r="G17" s="109">
-        <v>0</v>
-      </c>
-      <c r="H17" s="109">
-        <v>0</v>
-      </c>
-      <c r="I17" s="109">
-        <v>0</v>
-      </c>
-      <c r="J17" s="109">
-        <v>0</v>
-      </c>
-      <c r="K17" s="109">
-        <v>0</v>
-      </c>
-      <c r="L17" s="109">
-        <v>0</v>
-      </c>
-      <c r="M17" s="109">
-        <v>0</v>
-      </c>
-      <c r="N17" s="109">
-        <v>0</v>
-      </c>
-      <c r="O17" s="109">
-        <v>0</v>
-      </c>
-      <c r="P17" s="109">
-        <v>1.0000000000000002E-6</v>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0</v>
+      </c>
+      <c r="P17" s="1">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="109">
-        <v>0</v>
-      </c>
-      <c r="C18" s="109">
-        <v>0</v>
-      </c>
-      <c r="D18" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="E18" s="109">
-        <v>0</v>
-      </c>
-      <c r="F18" s="109">
-        <v>0</v>
-      </c>
-      <c r="G18" s="109">
-        <v>0</v>
-      </c>
-      <c r="H18" s="109">
-        <v>0</v>
-      </c>
-      <c r="I18" s="109">
-        <v>0</v>
-      </c>
-      <c r="J18" s="109">
-        <v>0</v>
-      </c>
-      <c r="K18" s="109">
-        <v>0</v>
-      </c>
-      <c r="L18" s="109">
-        <v>0</v>
-      </c>
-      <c r="M18" s="109">
-        <v>0</v>
-      </c>
-      <c r="N18" s="109">
-        <v>0</v>
-      </c>
-      <c r="O18" s="109">
-        <v>0</v>
-      </c>
-      <c r="P18" s="109">
-        <v>1.0000000000000002E-6</v>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="109">
-        <v>0</v>
-      </c>
-      <c r="C19" s="109">
-        <v>0</v>
-      </c>
-      <c r="D19" s="109">
-        <v>0</v>
-      </c>
-      <c r="E19" s="109">
-        <v>0</v>
-      </c>
-      <c r="F19" s="109">
-        <v>0</v>
-      </c>
-      <c r="G19" s="109">
-        <v>0</v>
-      </c>
-      <c r="H19" s="109">
-        <v>0</v>
-      </c>
-      <c r="I19" s="109">
-        <v>0</v>
-      </c>
-      <c r="J19" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="K19" s="109">
-        <v>0</v>
-      </c>
-      <c r="L19" s="109">
-        <v>0</v>
-      </c>
-      <c r="M19" s="109">
-        <v>0</v>
-      </c>
-      <c r="N19" s="109">
-        <v>0</v>
-      </c>
-      <c r="O19" s="109">
-        <v>0</v>
-      </c>
-      <c r="P19" s="109">
-        <v>1.0000000000000002E-6</v>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0</v>
+      </c>
+      <c r="P19" s="1">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="109">
-        <v>0</v>
-      </c>
-      <c r="C20" s="109">
-        <v>0</v>
-      </c>
-      <c r="D20" s="109">
-        <v>0</v>
-      </c>
-      <c r="E20" s="109">
-        <v>0</v>
-      </c>
-      <c r="F20" s="109">
-        <v>0</v>
-      </c>
-      <c r="G20" s="109">
-        <v>0</v>
-      </c>
-      <c r="H20" s="109">
-        <v>0</v>
-      </c>
-      <c r="I20" s="109">
-        <v>0</v>
-      </c>
-      <c r="J20" s="109">
-        <v>0</v>
-      </c>
-      <c r="K20" s="109">
-        <v>0</v>
-      </c>
-      <c r="L20" s="109">
-        <v>0</v>
-      </c>
-      <c r="M20" s="109">
-        <v>0</v>
-      </c>
-      <c r="N20" s="109">
-        <v>0</v>
-      </c>
-      <c r="O20" s="109">
-        <v>0</v>
-      </c>
-      <c r="P20" s="109">
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1">
         <v>0</v>
       </c>
     </row>
@@ -11153,49 +11158,49 @@
       <c r="A21" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="109">
-        <v>0</v>
-      </c>
-      <c r="C21" s="109">
-        <v>0</v>
-      </c>
-      <c r="D21" s="109">
-        <v>0</v>
-      </c>
-      <c r="E21" s="109">
-        <v>0</v>
-      </c>
-      <c r="F21" s="109">
-        <v>0</v>
-      </c>
-      <c r="G21" s="109">
-        <v>0</v>
-      </c>
-      <c r="H21" s="109">
-        <v>0</v>
-      </c>
-      <c r="I21" s="109">
-        <v>0</v>
-      </c>
-      <c r="J21" s="109">
-        <v>0</v>
-      </c>
-      <c r="K21" s="109">
-        <v>0</v>
-      </c>
-      <c r="L21" s="109">
-        <v>0</v>
-      </c>
-      <c r="M21" s="109">
-        <v>0</v>
-      </c>
-      <c r="N21" s="109">
-        <v>0</v>
-      </c>
-      <c r="O21" s="109">
-        <v>1.0000000000000002E-6</v>
-      </c>
-      <c r="P21" s="109">
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="P21" s="1">
         <v>0</v>
       </c>
     </row>
@@ -11214,14 +11219,14 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -11237,7 +11242,7 @@
         <v>117</v>
       </c>
       <c r="B3" s="29">
-        <v>1E-3</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -11252,15 +11257,15 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -11276,7 +11281,7 @@
         <v>117</v>
       </c>
       <c r="B3" s="29">
-        <v>1E-4</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -11292,7 +11297,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11304,7 +11309,7 @@
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Freshwater Souring Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Freshwater Souring Cost [kUSD/bbl]</v>
+        <v>Table of Freshwater Souring Cost [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -11320,7 +11325,7 @@
         <v>114</v>
       </c>
       <c r="B3" s="29">
-        <v>1.5E-3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -11328,7 +11333,7 @@
         <v>115</v>
       </c>
       <c r="B4" s="9">
-        <v>1.5499999999999999E-3</v>
+        <v>1.55</v>
       </c>
     </row>
   </sheetData>
@@ -11358,7 +11363,7 @@
     <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", "hour","]")</f>
-        <v>Table of Trucking Hourly Cost [kUSD/hour]</v>
+        <v>Table of Trucking Hourly Cost [USD/hour]</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -11594,7 +11599,7 @@
     <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),")]")</f>
-        <v>Table of Disposal Capacity Expansion Cost [kUSD/(bbl/day)]</v>
+        <v>Table of Disposal Capacity Expansion Cost [USD/(bbl/day)]</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -11666,7 +11671,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11747,7 +11752,7 @@
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Storage Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Storage Capacity Expansion Cost [kUSD/bbl]</v>
+        <v>Table of Storage Capacity Expansion Cost [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -11883,7 +11888,7 @@
     <row r="1" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Treatment Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),")]")</f>
-        <v>Table of Treatment Capacity Expansion Cost [kUSD/(bbl/day)]</v>
+        <v>Table of Treatment Capacity Expansion Cost [USD/(bbl/day)]</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -12272,7 +12277,7 @@
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Pipeline Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/(", VLOOKUP("diameter", Units!$A$2:$B$9, 2, FALSE),"-", VLOOKUP("distance", Units!$A$2:$B$9, 2, FALSE),")]")</f>
-        <v>Pipeline Expansion Cost [kUSD/(inch-mile)]</v>
+        <v>Pipeline Expansion Cost [USD/(inch-mile)]</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -13218,7 +13223,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13226,7 +13231,7 @@
     <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Pipeline Capacity Expansion Costs [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),")]")</f>
-        <v>Table of Pipeline Capacity Expansion Costs [kUSD/(bbl/day)]</v>
+        <v>Table of Pipeline Capacity Expansion Costs [USD/(bbl/day)]</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -13905,7 +13910,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -14025,7 +14030,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14284,8 +14289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC5B416-0D2D-42B4-AFE3-F87E08463FE6}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14295,8 +14300,8 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Freshwater Souring Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Freshwater Souring Cost [kUSD/bbl]</v>
+        <f>_xlfn.CONCAT( "Table of treatment revenue [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of treatment revenue [USD/bbl]</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -14312,15 +14317,15 @@
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B3" s="29">
-        <v>3.5E-4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B4" s="29">
         <v>0</v>

</xml_diff>